<commit_message>
ECP-1125: adds aggregation of general turnover aggregation properties
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/TurnoverImportForAggregated.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/TurnoverImportForAggregated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABFF209-12A1-714A-873D-23627FDDAE8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E668C5BF-F11A-1542-BAFE-335A2B930AAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32940" windowHeight="17900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="33820" windowHeight="20300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TurnoverImport" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="30">
   <si>
     <t>OXF-001</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>OXF-TOPMODEL-3</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>yyy</t>
+  </si>
+  <si>
+    <t>zzz</t>
   </si>
 </sst>
 </file>
@@ -754,7 +763,7 @@
   <dimension ref="A1:R77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1666,6 +1675,9 @@
       <c r="J26" s="6">
         <v>0</v>
       </c>
+      <c r="K26" t="s">
+        <v>27</v>
+      </c>
       <c r="L26" t="s">
         <v>3</v>
       </c>
@@ -1753,6 +1765,9 @@
       <c r="J29" s="6">
         <v>970</v>
       </c>
+      <c r="K29" t="s">
+        <v>28</v>
+      </c>
       <c r="L29" t="s">
         <v>3</v>
       </c>
@@ -2042,6 +2057,9 @@
       </c>
       <c r="J39" s="6">
         <v>532</v>
+      </c>
+      <c r="K39" t="s">
+        <v>29</v>
       </c>
       <c r="L39" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
ECP-1125: adds parallel occupancy scenario test
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/TurnoverImportForAggregated.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/TurnoverImportForAggregated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E668C5BF-F11A-1542-BAFE-335A2B930AAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB6AD13-7AD8-6940-9F53-2F3CCB384569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="460" windowWidth="33820" windowHeight="20300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="31">
   <si>
     <t>OXF-001</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>zzz</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -763,7 +766,7 @@
   <dimension ref="A1:R77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1444,6 +1447,9 @@
       <c r="J18" s="6">
         <v>120</v>
       </c>
+      <c r="K18" t="s">
+        <v>30</v>
+      </c>
       <c r="L18" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
ECP-1125: adds scenario parent leases
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/TurnoverImportForAggregated.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/TurnoverImportForAggregated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB6AD13-7AD8-6940-9F53-2F3CCB384569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68307463-E30D-7B41-9AD5-949CA525EA62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="33820" windowHeight="20300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33820" windowHeight="20300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TurnoverImport" sheetId="5" r:id="rId1"/>

</xml_diff>

<commit_message>
ECP-1125: first implementation for strategies SIMPLE and MANY_TO_ONE working
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/TurnoverImportForAggregated.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/TurnoverImportForAggregated.xlsx
@@ -8,15 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68307463-E30D-7B41-9AD5-949CA525EA62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978F18FA-62DF-E247-9C45-A73769B746A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33820" windowHeight="20300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TurnoverImport" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -766,7 +774,7 @@
   <dimension ref="A1:R77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
ECP-1125: adapts selection of configs to calculate and date range for aggregations
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/TurnoverImportForAggregated.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/TurnoverImportForAggregated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/turnoveraggregate/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978F18FA-62DF-E247-9C45-A73769B746A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C0C078-C9FB-134C-BDFB-B9286D60A481}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33820" windowHeight="20300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="30">
   <si>
     <t>OXF-001</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>OXF-TOPMODEL-3</t>
-  </si>
-  <si>
-    <t>xxx</t>
   </si>
   <si>
     <t>yyy</t>
@@ -774,7 +771,7 @@
   <dimension ref="A1:R77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1456,7 +1453,7 @@
         <v>120</v>
       </c>
       <c r="K18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L18" t="s">
         <v>3</v>
@@ -1689,9 +1686,6 @@
       <c r="J26" s="6">
         <v>0</v>
       </c>
-      <c r="K26" t="s">
-        <v>27</v>
-      </c>
       <c r="L26" t="s">
         <v>3</v>
       </c>
@@ -1780,7 +1774,7 @@
         <v>970</v>
       </c>
       <c r="K29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L29" t="s">
         <v>3</v>
@@ -2073,7 +2067,7 @@
         <v>532</v>
       </c>
       <c r="K39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L39" t="s">
         <v>3</v>

</xml_diff>